<commit_message>
Cambio botones escaner e inicio
</commit_message>
<xml_diff>
--- a/csv/Bares-TheGlass.xlsx
+++ b/csv/Bares-TheGlass.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Universidad\CM\TheGlass\csv\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A14F10-3CFB-4412-98DE-4D89F8721BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>nombre</t>
   </si>
@@ -156,13 +162,28 @@
   </si>
   <si>
     <t>10% con 150 puntos</t>
+  </si>
+  <si>
+    <t>CADA 5 EUROS</t>
+  </si>
+  <si>
+    <t>IMPORTE CUENTA</t>
+  </si>
+  <si>
+    <t>PUNTOS</t>
+  </si>
+  <si>
+    <t>TOTAL PUNTOS</t>
+  </si>
+  <si>
+    <t>EJEMPLOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -272,6 +293,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,30 +605,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -635,7 +662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -652,7 +679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -669,7 +696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -686,7 +713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -703,7 +730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -720,7 +747,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -737,7 +764,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -754,7 +781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -771,7 +798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -788,7 +815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -805,7 +832,82 @@
         <v>32</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f>A17*B17/5</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17.5</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C20" si="0">A18*B18/5</f>
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5.5</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:C15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>